<commit_message>
Updated SO Header and fulfillment TCs
</commit_message>
<xml_diff>
--- a/templates/QARSF/Parallel/SYDATA_Parallel_Allocate_PickPackShip.xlsx
+++ b/templates/QARSF/Parallel/SYDATA_Parallel_Allocate_PickPackShip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\WS_RSAutomation\rsqasampleproj\templates\QARSF\Parallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EAD9E7-4896-4E0F-9BA9-A88257AF4090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349266A3-3A08-4F2B-BB1F-D1A2244EC482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="761" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30315" yWindow="6660" windowWidth="15375" windowHeight="6435" tabRatio="761" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Allocate1" sheetId="5" r:id="rId1"/>
@@ -18,11 +18,16 @@
     <sheet name="Allocate3" sheetId="7" r:id="rId3"/>
     <sheet name="Allocate4" sheetId="8" r:id="rId4"/>
     <sheet name="Allocate5" sheetId="9" r:id="rId5"/>
-    <sheet name="PickPackShip1" sheetId="10" r:id="rId6"/>
-    <sheet name="PickPackShip2" sheetId="11" r:id="rId7"/>
-    <sheet name="PickPackShip3" sheetId="12" r:id="rId8"/>
-    <sheet name="PickPackShip4" sheetId="13" r:id="rId9"/>
-    <sheet name="PickPackShip5" sheetId="14" r:id="rId10"/>
+    <sheet name="Allocate6" sheetId="15" r:id="rId6"/>
+    <sheet name="Allocate7" sheetId="16" r:id="rId7"/>
+    <sheet name="Allocate8" sheetId="17" r:id="rId8"/>
+    <sheet name="Allocate9" sheetId="18" r:id="rId9"/>
+    <sheet name="Allocate10" sheetId="19" r:id="rId10"/>
+    <sheet name="PickPackShip1" sheetId="10" r:id="rId11"/>
+    <sheet name="PickPackShip2" sheetId="11" r:id="rId12"/>
+    <sheet name="PickPackShip3" sheetId="12" r:id="rId13"/>
+    <sheet name="PickPackShip4" sheetId="13" r:id="rId14"/>
+    <sheet name="PickPackShip5" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="53">
   <si>
     <t>Transaction Type</t>
   </si>
@@ -145,6 +150,63 @@
   </si>
   <si>
     <t>a5d1K000000SvbP</t>
+  </si>
+  <si>
+    <t>a5P1K000001ksYK</t>
+  </si>
+  <si>
+    <t>a5P1K000001ksYP</t>
+  </si>
+  <si>
+    <t>a5P1K000001ksYU</t>
+  </si>
+  <si>
+    <t>a5P1K000001ksYZ</t>
+  </si>
+  <si>
+    <t>a5P1K000001kvhtUAA</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32Q</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32R</t>
+  </si>
+  <si>
+    <t>a5P1K000001kvhyUAA</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32V</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32W</t>
+  </si>
+  <si>
+    <t>a5P1K000001kvi3UAA</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32a</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32b</t>
+  </si>
+  <si>
+    <t>a5P1K000001kvi8UAA</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32f</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32g</t>
+  </si>
+  <si>
+    <t>a5P1K000001kviDUAQ</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32k</t>
+  </si>
+  <si>
+    <t>a5d1K000000T32l</t>
   </si>
 </sst>
 </file>
@@ -495,7 +557,7 @@
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -566,11 +628,93 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33DAB0A-136A-47D0-9C2C-54C1993FD87F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B08887-17C4-4665-B71F-686E85306EF6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5D3B4-F28E-4A41-9365-29E1C70610E5}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,13 +756,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,13 +776,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -646,341 +790,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E645D2-136B-465B-B0E9-C79B11303BF0}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D741ABC-8364-4A18-98EF-00B808DF8D3C}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B243FA-2B41-4559-A187-32C186A7D846}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890B51B6-5023-4F92-8C17-A45A79B899F0}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C17CC05-5DCA-42E4-9D23-92CF173B7F60}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C5D3B4-F28E-4A41-9365-29E1C70610E5}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,13 +837,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1042,13 +857,13 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1056,88 +871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D741ABC-8364-4A18-98EF-00B808DF8D3C}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5D523D-6AD7-4F0A-A399-B0C07D681098}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1218,7 +952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AB6FCF-25A0-4575-A04C-1CA8838922B5}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1297,4 +1031,742 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33DAB0A-136A-47D0-9C2C-54C1993FD87F}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E645D2-136B-465B-B0E9-C79B11303BF0}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5B243FA-2B41-4559-A187-32C186A7D846}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890B51B6-5023-4F92-8C17-A45A79B899F0}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C17CC05-5DCA-42E4-9D23-92CF173B7F60}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A04DBE-8B53-4A58-83C4-6AFE8582067B}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDAC88E-6C1B-4EBC-BF56-8B608C939E71}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCE6433-DCEE-4B6D-8026-E9CC294C52C5}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D692130-2CBB-422D-AF1F-795E94F65CD0}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>